<commit_message>
Actualizado cuartos de final
</commit_message>
<xml_diff>
--- a/data/partidos/partidos_CESA25CF.xlsx
+++ b/data/partidos/partidos_CESA25CF.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:LP12"/>
+  <dimension ref="A1:LP16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7719,7 +7719,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>SELECCI? CATALANA CADET FEMENINA</t>
+          <t>SELECCION CANARIA CADETE FEMENINO</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -9331,7 +9331,7 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>SELECCI? CATALANA CADET FEMENINA</t>
+          <t>SELECCION CANARIA CADETE FEMENINO</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -10141,7 +10141,7 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>SELECCI? CATALANA CADET FEMENINA</t>
+          <t>SELECCION CANARIA CADETE FEMENINO</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -10925,6 +10925,3178 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1455946</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>06/01/2025</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>SEL. COMUNITAT VALENCIANA</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>ANDALUCIA CADETE FEMENINO</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>22</v>
+      </c>
+      <c r="I13" t="n">
+        <v>29</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4</v>
+      </c>
+      <c r="M13" t="n">
+        <v>5</v>
+      </c>
+      <c r="N13" t="n">
+        <v>8</v>
+      </c>
+      <c r="O13" t="n">
+        <v>6</v>
+      </c>
+      <c r="P13" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>7</v>
+      </c>
+      <c r="R13" t="n">
+        <v>11</v>
+      </c>
+      <c r="S13" t="n">
+        <v>8</v>
+      </c>
+      <c r="T13" t="n">
+        <v>12</v>
+      </c>
+      <c r="U13" t="n">
+        <v>11</v>
+      </c>
+      <c r="V13" t="n">
+        <v>13</v>
+      </c>
+      <c r="W13" t="n">
+        <v>14</v>
+      </c>
+      <c r="X13" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>21</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>29</v>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t>44:27</t>
+        </is>
+      </c>
+      <c r="AI13" t="inlineStr">
+        <is>
+          <t>20:20</t>
+        </is>
+      </c>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t>51:41</t>
+        </is>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>54:20</t>
+        </is>
+      </c>
+      <c r="AL13" t="inlineStr">
+        <is>
+          <t>51:49</t>
+        </is>
+      </c>
+      <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="inlineStr">
+        <is>
+          <t>LAURA ESCUDERO LEON</t>
+        </is>
+      </c>
+      <c r="AO13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP13" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
+      <c r="AR13" t="inlineStr"/>
+      <c r="AS13" t="inlineStr"/>
+      <c r="AT13" t="inlineStr"/>
+      <c r="AU13" t="inlineStr">
+        <is>
+          <t>AROA BELTRAN RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="AV13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW13" t="inlineStr"/>
+      <c r="AX13" t="inlineStr"/>
+      <c r="AY13" t="inlineStr"/>
+      <c r="AZ13" t="inlineStr"/>
+      <c r="BA13" t="inlineStr"/>
+      <c r="BB13" t="inlineStr">
+        <is>
+          <t>STASSY ADESUWA OKAFOR AMEN</t>
+        </is>
+      </c>
+      <c r="BC13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD13" t="inlineStr"/>
+      <c r="BE13" t="inlineStr"/>
+      <c r="BF13" t="inlineStr"/>
+      <c r="BG13" t="inlineStr"/>
+      <c r="BH13" t="inlineStr"/>
+      <c r="BI13" t="inlineStr">
+        <is>
+          <t>LAURA CONDE ESPINOSA</t>
+        </is>
+      </c>
+      <c r="BJ13" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK13" t="inlineStr"/>
+      <c r="BL13" t="inlineStr"/>
+      <c r="BM13" t="inlineStr"/>
+      <c r="BN13" t="inlineStr"/>
+      <c r="BO13" t="inlineStr"/>
+      <c r="BP13" t="inlineStr">
+        <is>
+          <t>ZULEMA ROMERO NAVARRO</t>
+        </is>
+      </c>
+      <c r="BQ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR13" t="inlineStr"/>
+      <c r="BS13" t="inlineStr"/>
+      <c r="BT13" t="inlineStr"/>
+      <c r="BU13" t="inlineStr"/>
+      <c r="BV13" t="inlineStr"/>
+      <c r="BW13" t="inlineStr">
+        <is>
+          <t>PAULA FERNANDEZ VERA</t>
+        </is>
+      </c>
+      <c r="BX13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BY13" t="inlineStr"/>
+      <c r="BZ13" t="inlineStr"/>
+      <c r="CA13" t="inlineStr"/>
+      <c r="CB13" t="inlineStr"/>
+      <c r="CC13" t="inlineStr"/>
+      <c r="CD13" t="inlineStr">
+        <is>
+          <t>CRISTINA IOANA TANCHI MICULAICIUC</t>
+        </is>
+      </c>
+      <c r="CE13" t="n">
+        <v>2</v>
+      </c>
+      <c r="CF13" t="inlineStr"/>
+      <c r="CG13" t="inlineStr"/>
+      <c r="CH13" t="inlineStr"/>
+      <c r="CI13" t="inlineStr"/>
+      <c r="CJ13" t="inlineStr"/>
+      <c r="CK13" t="inlineStr">
+        <is>
+          <t>SILVIA MARCELLO RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="CL13" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM13" t="inlineStr"/>
+      <c r="CN13" t="inlineStr"/>
+      <c r="CO13" t="inlineStr"/>
+      <c r="CP13" t="inlineStr"/>
+      <c r="CQ13" t="inlineStr"/>
+      <c r="CR13" t="inlineStr">
+        <is>
+          <t>ALEJANDRA APARICIO OLMOS</t>
+        </is>
+      </c>
+      <c r="CS13" t="n">
+        <v>1</v>
+      </c>
+      <c r="CT13" t="inlineStr"/>
+      <c r="CU13" t="inlineStr">
+        <is>
+          <t>36:32</t>
+        </is>
+      </c>
+      <c r="CV13" t="inlineStr"/>
+      <c r="CW13" t="inlineStr"/>
+      <c r="CX13" t="inlineStr"/>
+      <c r="CY13" t="inlineStr">
+        <is>
+          <t>DANIELA LEROY ORDOÑEZ</t>
+        </is>
+      </c>
+      <c r="CZ13" t="n">
+        <v>4</v>
+      </c>
+      <c r="DA13" t="inlineStr"/>
+      <c r="DB13" t="inlineStr">
+        <is>
+          <t>49:02</t>
+        </is>
+      </c>
+      <c r="DC13" t="inlineStr"/>
+      <c r="DD13" t="inlineStr"/>
+      <c r="DE13" t="inlineStr"/>
+      <c r="DF13" t="inlineStr">
+        <is>
+          <t>ADRIANA PORRAS GOMEZ</t>
+        </is>
+      </c>
+      <c r="DG13" t="n">
+        <v>0</v>
+      </c>
+      <c r="DH13" t="inlineStr"/>
+      <c r="DI13" t="inlineStr"/>
+      <c r="DJ13" t="inlineStr"/>
+      <c r="DK13" t="inlineStr"/>
+      <c r="DL13" t="inlineStr"/>
+      <c r="DM13" t="inlineStr">
+        <is>
+          <t>BEATRIZ BIEDMA GARRIDO</t>
+        </is>
+      </c>
+      <c r="DN13" t="n">
+        <v>7</v>
+      </c>
+      <c r="DO13" t="inlineStr"/>
+      <c r="DP13" t="inlineStr"/>
+      <c r="DQ13" t="inlineStr"/>
+      <c r="DR13" t="inlineStr"/>
+      <c r="DS13" t="inlineStr"/>
+      <c r="DT13" t="inlineStr">
+        <is>
+          <t>PAULA AGUADO MARTI</t>
+        </is>
+      </c>
+      <c r="DU13" t="n">
+        <v>1</v>
+      </c>
+      <c r="DV13" t="inlineStr"/>
+      <c r="DW13" t="inlineStr"/>
+      <c r="DX13" t="inlineStr"/>
+      <c r="DY13" t="inlineStr"/>
+      <c r="DZ13" t="inlineStr"/>
+      <c r="EA13" t="inlineStr">
+        <is>
+          <t>MARTA BOUZO ALONSO</t>
+        </is>
+      </c>
+      <c r="EB13" t="n">
+        <v>0</v>
+      </c>
+      <c r="EC13" t="inlineStr"/>
+      <c r="ED13" t="inlineStr"/>
+      <c r="EE13" t="inlineStr"/>
+      <c r="EF13" t="inlineStr"/>
+      <c r="EG13" t="inlineStr"/>
+      <c r="EH13" t="inlineStr">
+        <is>
+          <t>NOA LLOPIS IBAÑEZ</t>
+        </is>
+      </c>
+      <c r="EI13" t="n">
+        <v>2</v>
+      </c>
+      <c r="EJ13" t="inlineStr">
+        <is>
+          <t>02:24</t>
+        </is>
+      </c>
+      <c r="EK13" t="inlineStr"/>
+      <c r="EL13" t="inlineStr"/>
+      <c r="EM13" t="inlineStr"/>
+      <c r="EN13" t="inlineStr"/>
+      <c r="EO13" t="inlineStr">
+        <is>
+          <t>VICTORIA GOMEZ GARCIA</t>
+        </is>
+      </c>
+      <c r="EP13" t="n">
+        <v>0</v>
+      </c>
+      <c r="EQ13" t="inlineStr"/>
+      <c r="ER13" t="inlineStr"/>
+      <c r="ES13" t="inlineStr"/>
+      <c r="ET13" t="inlineStr"/>
+      <c r="EU13" t="inlineStr"/>
+      <c r="EV13" t="inlineStr">
+        <is>
+          <t>ANDREA FERNANDEZ GOMEZ</t>
+        </is>
+      </c>
+      <c r="EW13" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX13" t="inlineStr"/>
+      <c r="EY13" t="inlineStr"/>
+      <c r="EZ13" t="inlineStr"/>
+      <c r="FA13" t="inlineStr"/>
+      <c r="FB13" t="inlineStr"/>
+      <c r="FC13" t="inlineStr">
+        <is>
+          <t>SOFIA JAIME SANCHEZ</t>
+        </is>
+      </c>
+      <c r="FD13" t="n">
+        <v>5</v>
+      </c>
+      <c r="FE13" t="inlineStr"/>
+      <c r="FF13" t="inlineStr">
+        <is>
+          <t>32:21</t>
+        </is>
+      </c>
+      <c r="FG13" t="inlineStr"/>
+      <c r="FH13" t="inlineStr"/>
+      <c r="FI13" t="inlineStr"/>
+      <c r="FJ13" t="inlineStr">
+        <is>
+          <t>LAURA FERRER CAROT</t>
+        </is>
+      </c>
+      <c r="FK13" t="n">
+        <v>10</v>
+      </c>
+      <c r="FL13" t="inlineStr"/>
+      <c r="FM13" t="inlineStr">
+        <is>
+          <t>50:01</t>
+        </is>
+      </c>
+      <c r="FN13" t="inlineStr"/>
+      <c r="FO13" t="inlineStr"/>
+      <c r="FP13" t="inlineStr"/>
+      <c r="FQ13" t="inlineStr">
+        <is>
+          <t>MARTINA NEGRON AGUILAR</t>
+        </is>
+      </c>
+      <c r="FR13" t="n">
+        <v>4</v>
+      </c>
+      <c r="FS13" t="inlineStr"/>
+      <c r="FT13" t="inlineStr">
+        <is>
+          <t>17:54</t>
+        </is>
+      </c>
+      <c r="FU13" t="inlineStr"/>
+      <c r="FV13" t="inlineStr"/>
+      <c r="FW13" t="inlineStr"/>
+      <c r="FX13" t="inlineStr">
+        <is>
+          <t>MICHELLE RICO JUAN</t>
+        </is>
+      </c>
+      <c r="FY13" t="n">
+        <v>0</v>
+      </c>
+      <c r="FZ13" t="inlineStr"/>
+      <c r="GA13" t="inlineStr"/>
+      <c r="GB13" t="inlineStr"/>
+      <c r="GC13" t="inlineStr"/>
+      <c r="GD13" t="inlineStr"/>
+      <c r="GE13" t="inlineStr">
+        <is>
+          <t>ANA JAIME SANCHEZ</t>
+        </is>
+      </c>
+      <c r="GF13" t="n">
+        <v>2</v>
+      </c>
+      <c r="GG13" t="inlineStr"/>
+      <c r="GH13" t="inlineStr">
+        <is>
+          <t>12:49</t>
+        </is>
+      </c>
+      <c r="GI13" t="inlineStr"/>
+      <c r="GJ13" t="inlineStr"/>
+      <c r="GK13" t="inlineStr"/>
+      <c r="GL13" t="inlineStr">
+        <is>
+          <t>CRISTINA MARTINEZ TORRES</t>
+        </is>
+      </c>
+      <c r="GM13" t="n">
+        <v>1</v>
+      </c>
+      <c r="GN13" t="inlineStr"/>
+      <c r="GO13" t="inlineStr">
+        <is>
+          <t>01:28</t>
+        </is>
+      </c>
+      <c r="GP13" t="inlineStr">
+        <is>
+          <t>08:34</t>
+        </is>
+      </c>
+      <c r="GQ13" t="inlineStr"/>
+      <c r="GR13" t="inlineStr"/>
+      <c r="GS13" t="inlineStr">
+        <is>
+          <t>AMELIA GOMEZ BERNAL</t>
+        </is>
+      </c>
+      <c r="GT13" t="n">
+        <v>3</v>
+      </c>
+      <c r="GU13" t="inlineStr">
+        <is>
+          <t>11:24</t>
+        </is>
+      </c>
+      <c r="GV13" t="inlineStr"/>
+      <c r="GW13" t="inlineStr"/>
+      <c r="GX13" t="inlineStr"/>
+      <c r="GY13" t="inlineStr"/>
+      <c r="GZ13" t="inlineStr">
+        <is>
+          <t>MAR NAVARRO POMER</t>
+        </is>
+      </c>
+      <c r="HA13" t="n">
+        <v>2</v>
+      </c>
+      <c r="HB13" t="inlineStr"/>
+      <c r="HC13" t="inlineStr"/>
+      <c r="HD13" t="inlineStr"/>
+      <c r="HE13" t="inlineStr"/>
+      <c r="HF13" t="inlineStr"/>
+      <c r="HG13" t="inlineStr">
+        <is>
+          <t>DANIELA MARFIL TORRES</t>
+        </is>
+      </c>
+      <c r="HH13" t="n">
+        <v>0</v>
+      </c>
+      <c r="HI13" t="inlineStr"/>
+      <c r="HJ13" t="inlineStr"/>
+      <c r="HK13" t="inlineStr"/>
+      <c r="HL13" t="inlineStr"/>
+      <c r="HM13" t="inlineStr"/>
+      <c r="HN13" t="inlineStr">
+        <is>
+          <t>YANIN PARRES DIAZ</t>
+        </is>
+      </c>
+      <c r="HO13" t="n">
+        <v>0</v>
+      </c>
+      <c r="HP13" t="inlineStr"/>
+      <c r="HQ13" t="inlineStr"/>
+      <c r="HR13" t="inlineStr"/>
+      <c r="HS13" t="inlineStr"/>
+      <c r="HT13" t="inlineStr"/>
+      <c r="HU13" t="inlineStr">
+        <is>
+          <t>MARTINA VILLALVA SANCHEZ</t>
+        </is>
+      </c>
+      <c r="HV13" t="n">
+        <v>0</v>
+      </c>
+      <c r="HW13" t="inlineStr"/>
+      <c r="HX13" t="inlineStr">
+        <is>
+          <t>13:23</t>
+        </is>
+      </c>
+      <c r="HY13" t="inlineStr"/>
+      <c r="HZ13" t="inlineStr"/>
+      <c r="IA13" t="inlineStr"/>
+      <c r="IB13" t="inlineStr">
+        <is>
+          <t>KEIRA SAN NARCISO SEGURA</t>
+        </is>
+      </c>
+      <c r="IC13" t="n">
+        <v>3</v>
+      </c>
+      <c r="ID13" t="inlineStr"/>
+      <c r="IE13" t="inlineStr"/>
+      <c r="IF13" t="inlineStr"/>
+      <c r="IG13" t="inlineStr"/>
+      <c r="IH13" t="inlineStr"/>
+      <c r="II13" t="inlineStr">
+        <is>
+          <t>LOURDES MARIA TEBA ALCAZAR</t>
+        </is>
+      </c>
+      <c r="IJ13" t="n">
+        <v>2</v>
+      </c>
+      <c r="IK13" t="inlineStr"/>
+      <c r="IL13" t="inlineStr"/>
+      <c r="IM13" t="inlineStr"/>
+      <c r="IN13" t="inlineStr"/>
+      <c r="IO13" t="inlineStr"/>
+      <c r="IP13" t="inlineStr">
+        <is>
+          <t>SONIA PASTOR CALLADO</t>
+        </is>
+      </c>
+      <c r="IQ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="IR13" t="inlineStr"/>
+      <c r="IS13" t="inlineStr"/>
+      <c r="IT13" t="inlineStr"/>
+      <c r="IU13" t="inlineStr"/>
+      <c r="IV13" t="inlineStr"/>
+      <c r="IW13" t="inlineStr">
+        <is>
+          <t>SOFIA GUTIERREZ LEON</t>
+        </is>
+      </c>
+      <c r="IX13" t="n">
+        <v>1</v>
+      </c>
+      <c r="IY13" t="inlineStr"/>
+      <c r="IZ13" t="inlineStr"/>
+      <c r="JA13" t="inlineStr"/>
+      <c r="JB13" t="inlineStr"/>
+      <c r="JC13" t="inlineStr"/>
+      <c r="JD13" t="inlineStr">
+        <is>
+          <t>ENTRENADOR</t>
+        </is>
+      </c>
+      <c r="JE13" t="inlineStr">
+        <is>
+          <t>NURIA CORBI GOMIS</t>
+        </is>
+      </c>
+      <c r="JF13" t="inlineStr"/>
+      <c r="JG13" t="inlineStr"/>
+      <c r="JH13" t="inlineStr">
+        <is>
+          <t>OFICIAL</t>
+        </is>
+      </c>
+      <c r="JI13" t="inlineStr">
+        <is>
+          <t>NURIA ANDREU SEMPERE</t>
+        </is>
+      </c>
+      <c r="JJ13" t="inlineStr"/>
+      <c r="JK13" t="inlineStr"/>
+      <c r="JL13" t="inlineStr">
+        <is>
+          <t>OFICIAL</t>
+        </is>
+      </c>
+      <c r="JM13" t="inlineStr">
+        <is>
+          <t>LAURA ARVIZA VALERO</t>
+        </is>
+      </c>
+      <c r="JN13" t="inlineStr"/>
+      <c r="JO13" t="inlineStr"/>
+      <c r="JP13" t="inlineStr"/>
+      <c r="JQ13" t="inlineStr"/>
+      <c r="JR13" t="inlineStr"/>
+      <c r="JS13" t="inlineStr"/>
+      <c r="JT13" t="inlineStr"/>
+      <c r="JU13" t="inlineStr"/>
+      <c r="JV13" t="inlineStr"/>
+      <c r="JW13" t="inlineStr"/>
+      <c r="JX13" t="n">
+        <v>51</v>
+      </c>
+      <c r="JY13" t="n">
+        <v>-7</v>
+      </c>
+      <c r="JZ13" t="n">
+        <v>7</v>
+      </c>
+      <c r="KA13" t="n">
+        <v>4</v>
+      </c>
+      <c r="KB13" t="n">
+        <v>5</v>
+      </c>
+      <c r="KC13" t="n">
+        <v>1</v>
+      </c>
+      <c r="KD13" t="n">
+        <v>2</v>
+      </c>
+      <c r="KE13" t="n">
+        <v>3</v>
+      </c>
+      <c r="KF13" t="n">
+        <v>3</v>
+      </c>
+      <c r="KG13" t="n">
+        <v>4</v>
+      </c>
+      <c r="KH13" t="n">
+        <v>1</v>
+      </c>
+      <c r="KI13" t="n">
+        <v>1</v>
+      </c>
+      <c r="KJ13" t="n">
+        <v>1</v>
+      </c>
+      <c r="KK13" t="n">
+        <v>2</v>
+      </c>
+      <c r="KL13" t="n">
+        <v>1</v>
+      </c>
+      <c r="KM13" t="n">
+        <v>1</v>
+      </c>
+      <c r="KN13" t="n">
+        <v>3</v>
+      </c>
+      <c r="KO13" t="n">
+        <v>1</v>
+      </c>
+      <c r="KP13" t="n">
+        <v>3</v>
+      </c>
+      <c r="KQ13" t="n">
+        <v>3</v>
+      </c>
+      <c r="KR13" t="n">
+        <v>2</v>
+      </c>
+      <c r="KS13" t="n">
+        <v>2</v>
+      </c>
+      <c r="KT13" t="n">
+        <v>4</v>
+      </c>
+      <c r="KU13" t="n">
+        <v>1</v>
+      </c>
+      <c r="KV13" t="n">
+        <v>1</v>
+      </c>
+      <c r="KW13" t="n">
+        <v>1</v>
+      </c>
+      <c r="KX13" t="n">
+        <v>4</v>
+      </c>
+      <c r="KY13" t="n">
+        <v>2</v>
+      </c>
+      <c r="KZ13" t="n">
+        <v>4</v>
+      </c>
+      <c r="LA13" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LB13" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LC13" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LD13" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LE13" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LF13" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LG13" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LH13" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LI13" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LJ13" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LK13" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LL13" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LM13" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LN13" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LO13" t="n">
+        <v>5</v>
+      </c>
+      <c r="LP13" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1455947</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>06/01/2025</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>11:15</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>SELECCION CASTILLA LA MANCHA CADETE FEM.</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>SELECCION CANARIA CADETE FEMENINO</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>36</v>
+      </c>
+      <c r="I14" t="n">
+        <v>28</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" t="n">
+        <v>3</v>
+      </c>
+      <c r="L14" t="n">
+        <v>5</v>
+      </c>
+      <c r="M14" t="n">
+        <v>4</v>
+      </c>
+      <c r="N14" t="n">
+        <v>9</v>
+      </c>
+      <c r="O14" t="n">
+        <v>4</v>
+      </c>
+      <c r="P14" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>8</v>
+      </c>
+      <c r="R14" t="n">
+        <v>16</v>
+      </c>
+      <c r="S14" t="n">
+        <v>13</v>
+      </c>
+      <c r="T14" t="n">
+        <v>20</v>
+      </c>
+      <c r="U14" t="n">
+        <v>16</v>
+      </c>
+      <c r="V14" t="n">
+        <v>23</v>
+      </c>
+      <c r="W14" t="n">
+        <v>16</v>
+      </c>
+      <c r="X14" t="n">
+        <v>27</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>20</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>36</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>28</v>
+      </c>
+      <c r="AH14" t="inlineStr">
+        <is>
+          <t>21:16:00</t>
+        </is>
+      </c>
+      <c r="AI14" t="inlineStr">
+        <is>
+          <t>11:21:00</t>
+        </is>
+      </c>
+      <c r="AJ14" t="inlineStr">
+        <is>
+          <t>51:48</t>
+        </is>
+      </c>
+      <c r="AK14" t="inlineStr">
+        <is>
+          <t>33:47</t>
+        </is>
+      </c>
+      <c r="AL14" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="inlineStr">
+        <is>
+          <t>INES FIGUERO ALFARO</t>
+        </is>
+      </c>
+      <c r="AO14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP14" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
+      <c r="AR14" t="inlineStr"/>
+      <c r="AS14" t="inlineStr"/>
+      <c r="AT14" t="inlineStr"/>
+      <c r="AU14" t="inlineStr">
+        <is>
+          <t>ROCIO GOEZ PEREZ</t>
+        </is>
+      </c>
+      <c r="AV14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW14" t="inlineStr"/>
+      <c r="AX14" t="inlineStr"/>
+      <c r="AY14" t="inlineStr"/>
+      <c r="AZ14" t="inlineStr"/>
+      <c r="BA14" t="inlineStr"/>
+      <c r="BB14" t="inlineStr">
+        <is>
+          <t>IRENE SANCHEZ MALAGON</t>
+        </is>
+      </c>
+      <c r="BC14" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD14" t="inlineStr"/>
+      <c r="BE14" t="inlineStr"/>
+      <c r="BF14" t="inlineStr"/>
+      <c r="BG14" t="inlineStr"/>
+      <c r="BH14" t="inlineStr"/>
+      <c r="BI14" t="inlineStr">
+        <is>
+          <t>OGHENEYOMA ORHONIGBE</t>
+        </is>
+      </c>
+      <c r="BJ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK14" t="inlineStr"/>
+      <c r="BL14" t="inlineStr"/>
+      <c r="BM14" t="inlineStr"/>
+      <c r="BN14" t="inlineStr"/>
+      <c r="BO14" t="inlineStr"/>
+      <c r="BP14" t="inlineStr">
+        <is>
+          <t>AROA HERRERA HERRAIZ</t>
+        </is>
+      </c>
+      <c r="BQ14" t="n">
+        <v>9</v>
+      </c>
+      <c r="BR14" t="inlineStr"/>
+      <c r="BS14" t="inlineStr"/>
+      <c r="BT14" t="inlineStr"/>
+      <c r="BU14" t="inlineStr"/>
+      <c r="BV14" t="inlineStr"/>
+      <c r="BW14" t="inlineStr">
+        <is>
+          <t>DAHIANA MARTINEZ BARRETO</t>
+        </is>
+      </c>
+      <c r="BX14" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY14" t="inlineStr"/>
+      <c r="BZ14" t="inlineStr"/>
+      <c r="CA14" t="inlineStr"/>
+      <c r="CB14" t="inlineStr"/>
+      <c r="CC14" t="inlineStr"/>
+      <c r="CD14" t="inlineStr">
+        <is>
+          <t>ALEXANDRA POBLETE VERDE</t>
+        </is>
+      </c>
+      <c r="CE14" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF14" t="inlineStr"/>
+      <c r="CG14" t="inlineStr"/>
+      <c r="CH14" t="inlineStr"/>
+      <c r="CI14" t="inlineStr"/>
+      <c r="CJ14" t="inlineStr"/>
+      <c r="CK14" t="inlineStr">
+        <is>
+          <t>NAJARA ANGELES GABALDON MERINO</t>
+        </is>
+      </c>
+      <c r="CL14" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM14" t="inlineStr"/>
+      <c r="CN14" t="inlineStr"/>
+      <c r="CO14" t="inlineStr"/>
+      <c r="CP14" t="inlineStr"/>
+      <c r="CQ14" t="inlineStr"/>
+      <c r="CR14" t="inlineStr">
+        <is>
+          <t>PAULA PULIDO ROJAS</t>
+        </is>
+      </c>
+      <c r="CS14" t="n">
+        <v>3</v>
+      </c>
+      <c r="CT14" t="inlineStr"/>
+      <c r="CU14" t="inlineStr"/>
+      <c r="CV14" t="inlineStr"/>
+      <c r="CW14" t="inlineStr"/>
+      <c r="CX14" t="inlineStr"/>
+      <c r="CY14" t="inlineStr">
+        <is>
+          <t>INGRID BARRACHINA TAVIO</t>
+        </is>
+      </c>
+      <c r="CZ14" t="n">
+        <v>1</v>
+      </c>
+      <c r="DA14" t="inlineStr"/>
+      <c r="DB14" t="inlineStr"/>
+      <c r="DC14" t="inlineStr"/>
+      <c r="DD14" t="inlineStr"/>
+      <c r="DE14" t="inlineStr"/>
+      <c r="DF14" t="inlineStr">
+        <is>
+          <t>NEREA JIMENEZ ACEDO</t>
+        </is>
+      </c>
+      <c r="DG14" t="n">
+        <v>1</v>
+      </c>
+      <c r="DH14" t="inlineStr"/>
+      <c r="DI14" t="inlineStr">
+        <is>
+          <t>16:57</t>
+        </is>
+      </c>
+      <c r="DJ14" t="inlineStr">
+        <is>
+          <t>54:18</t>
+        </is>
+      </c>
+      <c r="DK14" t="inlineStr"/>
+      <c r="DL14" t="inlineStr"/>
+      <c r="DM14" t="inlineStr">
+        <is>
+          <t>AMELIA ALEXIA GABALDON MERINO</t>
+        </is>
+      </c>
+      <c r="DN14" t="n">
+        <v>7</v>
+      </c>
+      <c r="DO14" t="inlineStr"/>
+      <c r="DP14" t="inlineStr">
+        <is>
+          <t>11:11</t>
+        </is>
+      </c>
+      <c r="DQ14" t="inlineStr"/>
+      <c r="DR14" t="inlineStr"/>
+      <c r="DS14" t="inlineStr"/>
+      <c r="DT14" t="inlineStr">
+        <is>
+          <t>TERESA ROZAS PATIÑO</t>
+        </is>
+      </c>
+      <c r="DU14" t="n">
+        <v>2</v>
+      </c>
+      <c r="DV14" t="inlineStr"/>
+      <c r="DW14" t="inlineStr"/>
+      <c r="DX14" t="inlineStr"/>
+      <c r="DY14" t="inlineStr"/>
+      <c r="DZ14" t="inlineStr"/>
+      <c r="EA14" t="inlineStr">
+        <is>
+          <t>LEIRE GONZALEZ INFANTE</t>
+        </is>
+      </c>
+      <c r="EB14" t="n">
+        <v>1</v>
+      </c>
+      <c r="EC14" t="inlineStr"/>
+      <c r="ED14" t="inlineStr"/>
+      <c r="EE14" t="inlineStr"/>
+      <c r="EF14" t="inlineStr"/>
+      <c r="EG14" t="inlineStr"/>
+      <c r="EH14" t="inlineStr">
+        <is>
+          <t>EMMA CANO MONTARROSO</t>
+        </is>
+      </c>
+      <c r="EI14" t="n">
+        <v>5</v>
+      </c>
+      <c r="EJ14" t="inlineStr"/>
+      <c r="EK14" t="inlineStr">
+        <is>
+          <t>00:35</t>
+        </is>
+      </c>
+      <c r="EL14" t="inlineStr"/>
+      <c r="EM14" t="inlineStr"/>
+      <c r="EN14" t="inlineStr"/>
+      <c r="EO14" t="inlineStr">
+        <is>
+          <t>AMAIA BARRACHINA TAVIO</t>
+        </is>
+      </c>
+      <c r="EP14" t="n">
+        <v>1</v>
+      </c>
+      <c r="EQ14" t="inlineStr"/>
+      <c r="ER14" t="inlineStr">
+        <is>
+          <t>48:16</t>
+        </is>
+      </c>
+      <c r="ES14" t="inlineStr"/>
+      <c r="ET14" t="inlineStr"/>
+      <c r="EU14" t="inlineStr"/>
+      <c r="EV14" t="inlineStr">
+        <is>
+          <t>ELENA ISLA FERNANDEZ</t>
+        </is>
+      </c>
+      <c r="EW14" t="n">
+        <v>3</v>
+      </c>
+      <c r="EX14" t="inlineStr"/>
+      <c r="EY14" t="inlineStr">
+        <is>
+          <t>34:44</t>
+        </is>
+      </c>
+      <c r="EZ14" t="inlineStr"/>
+      <c r="FA14" t="inlineStr"/>
+      <c r="FB14" t="inlineStr"/>
+      <c r="FC14" t="inlineStr">
+        <is>
+          <t>MARBELYS REYES GOMEZ</t>
+        </is>
+      </c>
+      <c r="FD14" t="n">
+        <v>4</v>
+      </c>
+      <c r="FE14" t="inlineStr"/>
+      <c r="FF14" t="inlineStr"/>
+      <c r="FG14" t="inlineStr"/>
+      <c r="FH14" t="inlineStr"/>
+      <c r="FI14" t="inlineStr"/>
+      <c r="FJ14" t="inlineStr">
+        <is>
+          <t>LAURA MARTIN-BUITRAGO MATEOS DE ARRIBA</t>
+        </is>
+      </c>
+      <c r="FK14" t="n">
+        <v>2</v>
+      </c>
+      <c r="FL14" t="inlineStr"/>
+      <c r="FM14" t="inlineStr"/>
+      <c r="FN14" t="inlineStr"/>
+      <c r="FO14" t="inlineStr"/>
+      <c r="FP14" t="inlineStr"/>
+      <c r="FQ14" t="inlineStr">
+        <is>
+          <t>MARTHA PADRON OLSSON</t>
+        </is>
+      </c>
+      <c r="FR14" t="n">
+        <v>8</v>
+      </c>
+      <c r="FS14" t="inlineStr"/>
+      <c r="FT14" t="inlineStr"/>
+      <c r="FU14" t="inlineStr"/>
+      <c r="FV14" t="inlineStr"/>
+      <c r="FW14" t="inlineStr"/>
+      <c r="FX14" t="inlineStr">
+        <is>
+          <t>ADRIANA PACHECO MONROY</t>
+        </is>
+      </c>
+      <c r="FY14" t="n">
+        <v>7</v>
+      </c>
+      <c r="FZ14" t="inlineStr"/>
+      <c r="GA14" t="inlineStr"/>
+      <c r="GB14" t="inlineStr"/>
+      <c r="GC14" t="inlineStr"/>
+      <c r="GD14" t="inlineStr"/>
+      <c r="GE14" t="inlineStr">
+        <is>
+          <t>MARTINA LEMES MESEGUER</t>
+        </is>
+      </c>
+      <c r="GF14" t="n">
+        <v>2</v>
+      </c>
+      <c r="GG14" t="inlineStr"/>
+      <c r="GH14" t="inlineStr"/>
+      <c r="GI14" t="inlineStr"/>
+      <c r="GJ14" t="inlineStr"/>
+      <c r="GK14" t="inlineStr"/>
+      <c r="GL14" t="inlineStr">
+        <is>
+          <t>ELENA GONZALEZ GALLEGO-NICASIO</t>
+        </is>
+      </c>
+      <c r="GM14" t="n">
+        <v>0</v>
+      </c>
+      <c r="GN14" t="inlineStr"/>
+      <c r="GO14" t="inlineStr"/>
+      <c r="GP14" t="inlineStr"/>
+      <c r="GQ14" t="inlineStr"/>
+      <c r="GR14" t="inlineStr"/>
+      <c r="GS14" t="inlineStr">
+        <is>
+          <t>ADRIANA REYES FARRAY</t>
+        </is>
+      </c>
+      <c r="GT14" t="n">
+        <v>1</v>
+      </c>
+      <c r="GU14" t="inlineStr"/>
+      <c r="GV14" t="inlineStr"/>
+      <c r="GW14" t="inlineStr"/>
+      <c r="GX14" t="inlineStr"/>
+      <c r="GY14" t="inlineStr"/>
+      <c r="GZ14" t="inlineStr">
+        <is>
+          <t>ANA GUITART COVIELLA</t>
+        </is>
+      </c>
+      <c r="HA14" t="n">
+        <v>0</v>
+      </c>
+      <c r="HB14" t="inlineStr"/>
+      <c r="HC14" t="inlineStr">
+        <is>
+          <t>22:41</t>
+        </is>
+      </c>
+      <c r="HD14" t="inlineStr"/>
+      <c r="HE14" t="inlineStr"/>
+      <c r="HF14" t="inlineStr"/>
+      <c r="HG14" t="inlineStr">
+        <is>
+          <t>OIHANE XERACH PEÑA PADILLA</t>
+        </is>
+      </c>
+      <c r="HH14" t="n">
+        <v>1</v>
+      </c>
+      <c r="HI14" t="inlineStr"/>
+      <c r="HJ14" t="inlineStr"/>
+      <c r="HK14" t="inlineStr"/>
+      <c r="HL14" t="inlineStr"/>
+      <c r="HM14" t="inlineStr"/>
+      <c r="HN14" t="inlineStr">
+        <is>
+          <t>MIRIAM CANDELAS SANCHEZ-CARNERERO</t>
+        </is>
+      </c>
+      <c r="HO14" t="n">
+        <v>2</v>
+      </c>
+      <c r="HP14" t="inlineStr"/>
+      <c r="HQ14" t="inlineStr"/>
+      <c r="HR14" t="inlineStr"/>
+      <c r="HS14" t="inlineStr"/>
+      <c r="HT14" t="inlineStr"/>
+      <c r="HU14" t="inlineStr">
+        <is>
+          <t>NEYSA CURBELO BRITO</t>
+        </is>
+      </c>
+      <c r="HV14" t="n">
+        <v>0</v>
+      </c>
+      <c r="HW14" t="inlineStr"/>
+      <c r="HX14" t="inlineStr"/>
+      <c r="HY14" t="inlineStr"/>
+      <c r="HZ14" t="inlineStr"/>
+      <c r="IA14" t="inlineStr"/>
+      <c r="IB14" t="inlineStr">
+        <is>
+          <t>GUADALUPE ARANDA MAESTRE</t>
+        </is>
+      </c>
+      <c r="IC14" t="n">
+        <v>0</v>
+      </c>
+      <c r="ID14" t="inlineStr"/>
+      <c r="IE14" t="inlineStr"/>
+      <c r="IF14" t="inlineStr"/>
+      <c r="IG14" t="inlineStr"/>
+      <c r="IH14" t="inlineStr"/>
+      <c r="II14" t="inlineStr"/>
+      <c r="IJ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="IK14" t="inlineStr"/>
+      <c r="IL14" t="inlineStr"/>
+      <c r="IM14" t="inlineStr"/>
+      <c r="IN14" t="inlineStr"/>
+      <c r="IO14" t="inlineStr"/>
+      <c r="IP14" t="inlineStr">
+        <is>
+          <t>CAROLINA TORIBIO ASENSIO</t>
+        </is>
+      </c>
+      <c r="IQ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="IR14" t="inlineStr"/>
+      <c r="IS14" t="inlineStr"/>
+      <c r="IT14" t="inlineStr"/>
+      <c r="IU14" t="inlineStr"/>
+      <c r="IV14" t="inlineStr"/>
+      <c r="IW14" t="inlineStr"/>
+      <c r="IX14" t="n">
+        <v>0</v>
+      </c>
+      <c r="IY14" t="inlineStr"/>
+      <c r="IZ14" t="inlineStr"/>
+      <c r="JA14" t="inlineStr"/>
+      <c r="JB14" t="inlineStr"/>
+      <c r="JC14" t="inlineStr"/>
+      <c r="JD14" t="inlineStr">
+        <is>
+          <t>ENTRENADOR</t>
+        </is>
+      </c>
+      <c r="JE14" t="inlineStr">
+        <is>
+          <t>CARLOS CRUZ DE LA RUBIA</t>
+        </is>
+      </c>
+      <c r="JF14" t="inlineStr"/>
+      <c r="JG14" t="inlineStr"/>
+      <c r="JH14" t="inlineStr">
+        <is>
+          <t>AYTE ENTRENADOR</t>
+        </is>
+      </c>
+      <c r="JI14" t="inlineStr">
+        <is>
+          <t>ALBA AFONSO CASTRO</t>
+        </is>
+      </c>
+      <c r="JJ14" t="inlineStr"/>
+      <c r="JK14" t="inlineStr"/>
+      <c r="JL14" t="inlineStr">
+        <is>
+          <t>OFICIAL</t>
+        </is>
+      </c>
+      <c r="JM14" t="inlineStr">
+        <is>
+          <t>GONZALO LOPEZ-TOLA RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="JN14" t="inlineStr"/>
+      <c r="JO14" t="inlineStr"/>
+      <c r="JP14" t="inlineStr">
+        <is>
+          <t>OFICIAL</t>
+        </is>
+      </c>
+      <c r="JQ14" t="inlineStr">
+        <is>
+          <t>CRISTIAN MANTECON CAMPOS</t>
+        </is>
+      </c>
+      <c r="JR14" t="inlineStr"/>
+      <c r="JS14" t="inlineStr"/>
+      <c r="JT14" t="inlineStr"/>
+      <c r="JU14" t="inlineStr"/>
+      <c r="JV14" t="inlineStr"/>
+      <c r="JW14" t="inlineStr"/>
+      <c r="JX14" t="n">
+        <v>64</v>
+      </c>
+      <c r="JY14" t="n">
+        <v>8</v>
+      </c>
+      <c r="JZ14" t="n">
+        <v>8</v>
+      </c>
+      <c r="KA14" t="n">
+        <v>5</v>
+      </c>
+      <c r="KB14" t="n">
+        <v>2</v>
+      </c>
+      <c r="KC14" t="n">
+        <v>2</v>
+      </c>
+      <c r="KD14" t="n">
+        <v>3</v>
+      </c>
+      <c r="KE14" t="n">
+        <v>3</v>
+      </c>
+      <c r="KF14" t="n">
+        <v>1</v>
+      </c>
+      <c r="KG14" t="n">
+        <v>4</v>
+      </c>
+      <c r="KH14" t="n">
+        <v>0</v>
+      </c>
+      <c r="KI14" t="n">
+        <v>4</v>
+      </c>
+      <c r="KJ14" t="n">
+        <v>4</v>
+      </c>
+      <c r="KK14" t="n">
+        <v>3</v>
+      </c>
+      <c r="KL14" t="n">
+        <v>5</v>
+      </c>
+      <c r="KM14" t="n">
+        <v>4</v>
+      </c>
+      <c r="KN14" t="n">
+        <v>3</v>
+      </c>
+      <c r="KO14" t="n">
+        <v>3</v>
+      </c>
+      <c r="KP14" t="n">
+        <v>0</v>
+      </c>
+      <c r="KQ14" t="n">
+        <v>4</v>
+      </c>
+      <c r="KR14" t="n">
+        <v>4</v>
+      </c>
+      <c r="KS14" t="n">
+        <v>1</v>
+      </c>
+      <c r="KT14" t="n">
+        <v>1</v>
+      </c>
+      <c r="KU14" t="n">
+        <v>1</v>
+      </c>
+      <c r="KV14" t="n">
+        <v>1</v>
+      </c>
+      <c r="KW14" t="n">
+        <v>3</v>
+      </c>
+      <c r="KX14" t="n">
+        <v>3</v>
+      </c>
+      <c r="KY14" t="n">
+        <v>4</v>
+      </c>
+      <c r="KZ14" t="n">
+        <v>3</v>
+      </c>
+      <c r="LA14" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LB14" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LC14" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LD14" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LE14" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LF14" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LG14" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LH14" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LI14" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LJ14" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LK14" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LL14" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LM14" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LN14" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LO14" t="n">
+        <v>5</v>
+      </c>
+      <c r="LP14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1455948</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>06/01/2025</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>SEL. NAVARRA CADETE FEMENINO</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Seleccion de Euskadi Cadete Femenina</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>34</v>
+      </c>
+      <c r="I15" t="n">
+        <v>30</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2</v>
+      </c>
+      <c r="K15" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" t="n">
+        <v>5</v>
+      </c>
+      <c r="M15" t="n">
+        <v>5</v>
+      </c>
+      <c r="N15" t="n">
+        <v>9</v>
+      </c>
+      <c r="O15" t="n">
+        <v>8</v>
+      </c>
+      <c r="P15" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>9</v>
+      </c>
+      <c r="R15" t="n">
+        <v>18</v>
+      </c>
+      <c r="S15" t="n">
+        <v>12</v>
+      </c>
+      <c r="T15" t="n">
+        <v>20</v>
+      </c>
+      <c r="U15" t="n">
+        <v>14</v>
+      </c>
+      <c r="V15" t="n">
+        <v>23</v>
+      </c>
+      <c r="W15" t="n">
+        <v>16</v>
+      </c>
+      <c r="X15" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>18</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>28</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>34</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>30</v>
+      </c>
+      <c r="AH15" t="inlineStr">
+        <is>
+          <t>28:16</t>
+        </is>
+      </c>
+      <c r="AI15" t="inlineStr">
+        <is>
+          <t>16:28</t>
+        </is>
+      </c>
+      <c r="AJ15" t="inlineStr">
+        <is>
+          <t>46:26</t>
+        </is>
+      </c>
+      <c r="AK15" t="inlineStr"/>
+      <c r="AL15" t="inlineStr"/>
+      <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr">
+        <is>
+          <t>MIREN VALLES BONAFONTE</t>
+        </is>
+      </c>
+      <c r="AO15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP15" t="inlineStr"/>
+      <c r="AQ15" t="inlineStr"/>
+      <c r="AR15" t="inlineStr"/>
+      <c r="AS15" t="inlineStr"/>
+      <c r="AT15" t="inlineStr"/>
+      <c r="AU15" t="inlineStr">
+        <is>
+          <t>LORE URIBE ARIAS</t>
+        </is>
+      </c>
+      <c r="AV15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW15" t="inlineStr"/>
+      <c r="AX15" t="inlineStr"/>
+      <c r="AY15" t="inlineStr"/>
+      <c r="AZ15" t="inlineStr"/>
+      <c r="BA15" t="inlineStr"/>
+      <c r="BB15" t="inlineStr">
+        <is>
+          <t>SONIA CAÑADA PEREZ</t>
+        </is>
+      </c>
+      <c r="BC15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD15" t="inlineStr"/>
+      <c r="BE15" t="inlineStr"/>
+      <c r="BF15" t="inlineStr"/>
+      <c r="BG15" t="inlineStr"/>
+      <c r="BH15" t="inlineStr"/>
+      <c r="BI15" t="inlineStr">
+        <is>
+          <t>MALEN SUAREZ LOPEZ</t>
+        </is>
+      </c>
+      <c r="BJ15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK15" t="inlineStr"/>
+      <c r="BL15" t="inlineStr"/>
+      <c r="BM15" t="inlineStr"/>
+      <c r="BN15" t="inlineStr"/>
+      <c r="BO15" t="inlineStr"/>
+      <c r="BP15" t="inlineStr">
+        <is>
+          <t>AMAIA ARANGUREN ZALBA</t>
+        </is>
+      </c>
+      <c r="BQ15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR15" t="inlineStr"/>
+      <c r="BS15" t="inlineStr"/>
+      <c r="BT15" t="inlineStr"/>
+      <c r="BU15" t="inlineStr"/>
+      <c r="BV15" t="inlineStr"/>
+      <c r="BW15" t="inlineStr">
+        <is>
+          <t>AXUN GOMEZ ALBERDI</t>
+        </is>
+      </c>
+      <c r="BX15" t="n">
+        <v>2</v>
+      </c>
+      <c r="BY15" t="inlineStr"/>
+      <c r="BZ15" t="inlineStr">
+        <is>
+          <t>11:07</t>
+        </is>
+      </c>
+      <c r="CA15" t="inlineStr"/>
+      <c r="CB15" t="inlineStr"/>
+      <c r="CC15" t="inlineStr"/>
+      <c r="CD15" t="inlineStr">
+        <is>
+          <t>JULIA MENDINUETA FERNANDEZ</t>
+        </is>
+      </c>
+      <c r="CE15" t="n">
+        <v>7</v>
+      </c>
+      <c r="CF15" t="inlineStr"/>
+      <c r="CG15" t="inlineStr">
+        <is>
+          <t>04:26</t>
+        </is>
+      </c>
+      <c r="CH15" t="inlineStr">
+        <is>
+          <t>13:55</t>
+        </is>
+      </c>
+      <c r="CI15" t="inlineStr"/>
+      <c r="CJ15" t="inlineStr"/>
+      <c r="CK15" t="inlineStr">
+        <is>
+          <t>LIBE ALVAREZ MOYA</t>
+        </is>
+      </c>
+      <c r="CL15" t="n">
+        <v>4</v>
+      </c>
+      <c r="CM15" t="inlineStr"/>
+      <c r="CN15" t="inlineStr"/>
+      <c r="CO15" t="inlineStr"/>
+      <c r="CP15" t="inlineStr"/>
+      <c r="CQ15" t="inlineStr"/>
+      <c r="CR15" t="inlineStr">
+        <is>
+          <t>IRATI OLORIZ OLLO</t>
+        </is>
+      </c>
+      <c r="CS15" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT15" t="inlineStr"/>
+      <c r="CU15" t="inlineStr"/>
+      <c r="CV15" t="inlineStr"/>
+      <c r="CW15" t="inlineStr"/>
+      <c r="CX15" t="inlineStr"/>
+      <c r="CY15" t="inlineStr">
+        <is>
+          <t>PAULA DIAZ PAUL</t>
+        </is>
+      </c>
+      <c r="CZ15" t="n">
+        <v>0</v>
+      </c>
+      <c r="DA15" t="inlineStr"/>
+      <c r="DB15" t="inlineStr"/>
+      <c r="DC15" t="inlineStr"/>
+      <c r="DD15" t="inlineStr"/>
+      <c r="DE15" t="inlineStr"/>
+      <c r="DF15" t="inlineStr">
+        <is>
+          <t>JUNE CASIMIRO SALAS</t>
+        </is>
+      </c>
+      <c r="DG15" t="n">
+        <v>1</v>
+      </c>
+      <c r="DH15" t="inlineStr"/>
+      <c r="DI15" t="inlineStr"/>
+      <c r="DJ15" t="inlineStr"/>
+      <c r="DK15" t="inlineStr"/>
+      <c r="DL15" t="inlineStr"/>
+      <c r="DM15" t="inlineStr">
+        <is>
+          <t>OLAITZ LANDERA UNIBASO</t>
+        </is>
+      </c>
+      <c r="DN15" t="n">
+        <v>3</v>
+      </c>
+      <c r="DO15" t="inlineStr"/>
+      <c r="DP15" t="inlineStr"/>
+      <c r="DQ15" t="inlineStr"/>
+      <c r="DR15" t="inlineStr"/>
+      <c r="DS15" t="inlineStr"/>
+      <c r="DT15" t="inlineStr">
+        <is>
+          <t>KATTALIN ECHEGARAY VIGURIA</t>
+        </is>
+      </c>
+      <c r="DU15" t="n">
+        <v>6</v>
+      </c>
+      <c r="DV15" t="inlineStr"/>
+      <c r="DW15" t="inlineStr"/>
+      <c r="DX15" t="inlineStr"/>
+      <c r="DY15" t="inlineStr"/>
+      <c r="DZ15" t="inlineStr"/>
+      <c r="EA15" t="inlineStr">
+        <is>
+          <t>NOA IZAGUIRRE GOMEZ</t>
+        </is>
+      </c>
+      <c r="EB15" t="n">
+        <v>1</v>
+      </c>
+      <c r="EC15" t="inlineStr"/>
+      <c r="ED15" t="inlineStr"/>
+      <c r="EE15" t="inlineStr"/>
+      <c r="EF15" t="inlineStr"/>
+      <c r="EG15" t="inlineStr"/>
+      <c r="EH15" t="inlineStr">
+        <is>
+          <t>ANNE BELOKI LARRAYA</t>
+        </is>
+      </c>
+      <c r="EI15" t="n">
+        <v>4</v>
+      </c>
+      <c r="EJ15" t="inlineStr"/>
+      <c r="EK15" t="inlineStr">
+        <is>
+          <t>35:58</t>
+        </is>
+      </c>
+      <c r="EL15" t="inlineStr"/>
+      <c r="EM15" t="inlineStr"/>
+      <c r="EN15" t="inlineStr"/>
+      <c r="EO15" t="inlineStr">
+        <is>
+          <t>MAIALEN KERR ELGUEZUA</t>
+        </is>
+      </c>
+      <c r="EP15" t="n">
+        <v>1</v>
+      </c>
+      <c r="EQ15" t="inlineStr"/>
+      <c r="ER15" t="inlineStr"/>
+      <c r="ES15" t="inlineStr"/>
+      <c r="ET15" t="inlineStr"/>
+      <c r="EU15" t="inlineStr"/>
+      <c r="EV15" t="inlineStr">
+        <is>
+          <t>MARTA ESLAVA IBARROLA</t>
+        </is>
+      </c>
+      <c r="EW15" t="n">
+        <v>1</v>
+      </c>
+      <c r="EX15" t="inlineStr"/>
+      <c r="EY15" t="inlineStr"/>
+      <c r="EZ15" t="inlineStr"/>
+      <c r="FA15" t="inlineStr"/>
+      <c r="FB15" t="inlineStr"/>
+      <c r="FC15" t="inlineStr">
+        <is>
+          <t>IRAIA BERROETA SANCHEZ</t>
+        </is>
+      </c>
+      <c r="FD15" t="n">
+        <v>5</v>
+      </c>
+      <c r="FE15" t="inlineStr"/>
+      <c r="FF15" t="inlineStr">
+        <is>
+          <t>43:54</t>
+        </is>
+      </c>
+      <c r="FG15" t="inlineStr"/>
+      <c r="FH15" t="inlineStr"/>
+      <c r="FI15" t="inlineStr"/>
+      <c r="FJ15" t="inlineStr">
+        <is>
+          <t>CARLOTA CHIVITE FALCON</t>
+        </is>
+      </c>
+      <c r="FK15" t="n">
+        <v>4</v>
+      </c>
+      <c r="FL15" t="inlineStr"/>
+      <c r="FM15" t="inlineStr"/>
+      <c r="FN15" t="inlineStr"/>
+      <c r="FO15" t="inlineStr"/>
+      <c r="FP15" t="inlineStr"/>
+      <c r="FQ15" t="inlineStr">
+        <is>
+          <t>SARE AGUIRREZABAL ZARATE</t>
+        </is>
+      </c>
+      <c r="FR15" t="n">
+        <v>0</v>
+      </c>
+      <c r="FS15" t="inlineStr"/>
+      <c r="FT15" t="inlineStr"/>
+      <c r="FU15" t="inlineStr"/>
+      <c r="FV15" t="inlineStr"/>
+      <c r="FW15" t="inlineStr"/>
+      <c r="FX15" t="inlineStr">
+        <is>
+          <t>LEYRE MANRIQUE BIAIN</t>
+        </is>
+      </c>
+      <c r="FY15" t="n">
+        <v>0</v>
+      </c>
+      <c r="FZ15" t="inlineStr"/>
+      <c r="GA15" t="inlineStr"/>
+      <c r="GB15" t="inlineStr"/>
+      <c r="GC15" t="inlineStr"/>
+      <c r="GD15" t="inlineStr"/>
+      <c r="GE15" t="inlineStr">
+        <is>
+          <t>AMAIA CAMARERO AREVALO</t>
+        </is>
+      </c>
+      <c r="GF15" t="n">
+        <v>2</v>
+      </c>
+      <c r="GG15" t="inlineStr"/>
+      <c r="GH15" t="inlineStr"/>
+      <c r="GI15" t="inlineStr"/>
+      <c r="GJ15" t="inlineStr"/>
+      <c r="GK15" t="inlineStr"/>
+      <c r="GL15" t="inlineStr">
+        <is>
+          <t>IRENE GLARIA SANZ</t>
+        </is>
+      </c>
+      <c r="GM15" t="n">
+        <v>4</v>
+      </c>
+      <c r="GN15" t="inlineStr"/>
+      <c r="GO15" t="inlineStr">
+        <is>
+          <t>53:26</t>
+        </is>
+      </c>
+      <c r="GP15" t="inlineStr"/>
+      <c r="GQ15" t="inlineStr"/>
+      <c r="GR15" t="inlineStr"/>
+      <c r="GS15" t="inlineStr">
+        <is>
+          <t>MARA ZUBIZARRETA CABALLERO</t>
+        </is>
+      </c>
+      <c r="GT15" t="n">
+        <v>2</v>
+      </c>
+      <c r="GU15" t="inlineStr"/>
+      <c r="GV15" t="inlineStr"/>
+      <c r="GW15" t="inlineStr"/>
+      <c r="GX15" t="inlineStr"/>
+      <c r="GY15" t="inlineStr"/>
+      <c r="GZ15" t="inlineStr">
+        <is>
+          <t>IRUNE ARRASATE CASIMIRO</t>
+        </is>
+      </c>
+      <c r="HA15" t="n">
+        <v>1</v>
+      </c>
+      <c r="HB15" t="inlineStr"/>
+      <c r="HC15" t="inlineStr"/>
+      <c r="HD15" t="inlineStr"/>
+      <c r="HE15" t="inlineStr"/>
+      <c r="HF15" t="inlineStr"/>
+      <c r="HG15" t="inlineStr">
+        <is>
+          <t>JANIRE MARINA ABRALDES</t>
+        </is>
+      </c>
+      <c r="HH15" t="n">
+        <v>3</v>
+      </c>
+      <c r="HI15" t="inlineStr"/>
+      <c r="HJ15" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="HK15" t="inlineStr"/>
+      <c r="HL15" t="inlineStr"/>
+      <c r="HM15" t="inlineStr"/>
+      <c r="HN15" t="inlineStr">
+        <is>
+          <t>INES GARCIA ORDUÑA</t>
+        </is>
+      </c>
+      <c r="HO15" t="n">
+        <v>3</v>
+      </c>
+      <c r="HP15" t="inlineStr"/>
+      <c r="HQ15" t="inlineStr"/>
+      <c r="HR15" t="inlineStr"/>
+      <c r="HS15" t="inlineStr"/>
+      <c r="HT15" t="inlineStr"/>
+      <c r="HU15" t="inlineStr">
+        <is>
+          <t>MIREIA URBIETA MANTEROLA</t>
+        </is>
+      </c>
+      <c r="HV15" t="n">
+        <v>1</v>
+      </c>
+      <c r="HW15" t="inlineStr"/>
+      <c r="HX15" t="inlineStr">
+        <is>
+          <t>52:42</t>
+        </is>
+      </c>
+      <c r="HY15" t="inlineStr"/>
+      <c r="HZ15" t="inlineStr"/>
+      <c r="IA15" t="inlineStr"/>
+      <c r="IB15" t="inlineStr">
+        <is>
+          <t>UXUE BUSTO ALONSO</t>
+        </is>
+      </c>
+      <c r="IC15" t="n">
+        <v>2</v>
+      </c>
+      <c r="ID15" t="inlineStr"/>
+      <c r="IE15" t="inlineStr"/>
+      <c r="IF15" t="inlineStr"/>
+      <c r="IG15" t="inlineStr"/>
+      <c r="IH15" t="inlineStr"/>
+      <c r="II15" t="inlineStr">
+        <is>
+          <t>KIRA LOPEZ GALARRAGA</t>
+        </is>
+      </c>
+      <c r="IJ15" t="n">
+        <v>0</v>
+      </c>
+      <c r="IK15" t="inlineStr"/>
+      <c r="IL15" t="inlineStr">
+        <is>
+          <t>22:41</t>
+        </is>
+      </c>
+      <c r="IM15" t="inlineStr"/>
+      <c r="IN15" t="inlineStr"/>
+      <c r="IO15" t="inlineStr"/>
+      <c r="IP15" t="inlineStr">
+        <is>
+          <t>IRUNE CILVETI VEGUILLAS</t>
+        </is>
+      </c>
+      <c r="IQ15" t="n">
+        <v>1</v>
+      </c>
+      <c r="IR15" t="inlineStr"/>
+      <c r="IS15" t="inlineStr"/>
+      <c r="IT15" t="inlineStr"/>
+      <c r="IU15" t="inlineStr"/>
+      <c r="IV15" t="inlineStr"/>
+      <c r="IW15" t="inlineStr">
+        <is>
+          <t>MARTINA MARQUINEZ FERNANDEZ</t>
+        </is>
+      </c>
+      <c r="IX15" t="n">
+        <v>6</v>
+      </c>
+      <c r="IY15" t="inlineStr"/>
+      <c r="IZ15" t="inlineStr"/>
+      <c r="JA15" t="inlineStr"/>
+      <c r="JB15" t="inlineStr"/>
+      <c r="JC15" t="inlineStr"/>
+      <c r="JD15" t="inlineStr">
+        <is>
+          <t>ENTRENADOR</t>
+        </is>
+      </c>
+      <c r="JE15" t="inlineStr">
+        <is>
+          <t>OSCAR PASCUAL SILANES</t>
+        </is>
+      </c>
+      <c r="JF15" t="inlineStr"/>
+      <c r="JG15" t="inlineStr"/>
+      <c r="JH15" t="inlineStr">
+        <is>
+          <t>AYTE ENTRENADOR</t>
+        </is>
+      </c>
+      <c r="JI15" t="inlineStr">
+        <is>
+          <t>JAIME MORACHO GARNICA</t>
+        </is>
+      </c>
+      <c r="JJ15" t="inlineStr"/>
+      <c r="JK15" t="inlineStr"/>
+      <c r="JL15" t="inlineStr">
+        <is>
+          <t>OFICIAL</t>
+        </is>
+      </c>
+      <c r="JM15" t="inlineStr">
+        <is>
+          <t>GORKA METAXAS CHOCARRO</t>
+        </is>
+      </c>
+      <c r="JN15" t="inlineStr"/>
+      <c r="JO15" t="inlineStr"/>
+      <c r="JP15" t="inlineStr">
+        <is>
+          <t>OFICIAL</t>
+        </is>
+      </c>
+      <c r="JQ15" t="inlineStr">
+        <is>
+          <t>AINHOA FUENTE ESLAVA</t>
+        </is>
+      </c>
+      <c r="JR15" t="inlineStr"/>
+      <c r="JS15" t="inlineStr"/>
+      <c r="JT15" t="inlineStr"/>
+      <c r="JU15" t="inlineStr"/>
+      <c r="JV15" t="inlineStr"/>
+      <c r="JW15" t="inlineStr"/>
+      <c r="JX15" t="n">
+        <v>64</v>
+      </c>
+      <c r="JY15" t="n">
+        <v>4</v>
+      </c>
+      <c r="JZ15" t="n">
+        <v>4</v>
+      </c>
+      <c r="KA15" t="n">
+        <v>4</v>
+      </c>
+      <c r="KB15" t="n">
+        <v>5</v>
+      </c>
+      <c r="KC15" t="n">
+        <v>2</v>
+      </c>
+      <c r="KD15" t="n">
+        <v>3</v>
+      </c>
+      <c r="KE15" t="n">
+        <v>3</v>
+      </c>
+      <c r="KF15" t="n">
+        <v>2</v>
+      </c>
+      <c r="KG15" t="n">
+        <v>4</v>
+      </c>
+      <c r="KH15" t="n">
+        <v>3</v>
+      </c>
+      <c r="KI15" t="n">
+        <v>4</v>
+      </c>
+      <c r="KJ15" t="n">
+        <v>1</v>
+      </c>
+      <c r="KK15" t="n">
+        <v>5</v>
+      </c>
+      <c r="KL15" t="n">
+        <v>3</v>
+      </c>
+      <c r="KM15" t="n">
+        <v>2</v>
+      </c>
+      <c r="KN15" t="n">
+        <v>2</v>
+      </c>
+      <c r="KO15" t="n">
+        <v>3</v>
+      </c>
+      <c r="KP15" t="n">
+        <v>2</v>
+      </c>
+      <c r="KQ15" t="n">
+        <v>2</v>
+      </c>
+      <c r="KR15" t="n">
+        <v>2</v>
+      </c>
+      <c r="KS15" t="n">
+        <v>0</v>
+      </c>
+      <c r="KT15" t="n">
+        <v>3</v>
+      </c>
+      <c r="KU15" t="n">
+        <v>4</v>
+      </c>
+      <c r="KV15" t="n">
+        <v>5</v>
+      </c>
+      <c r="KW15" t="n">
+        <v>3</v>
+      </c>
+      <c r="KX15" t="n">
+        <v>2</v>
+      </c>
+      <c r="KY15" t="n">
+        <v>2</v>
+      </c>
+      <c r="KZ15" t="n">
+        <v>2</v>
+      </c>
+      <c r="LA15" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LB15" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LC15" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LD15" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LE15" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LF15" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LG15" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LH15" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LI15" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LJ15" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LK15" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LL15" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LM15" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LN15" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LO15" t="n">
+        <v>4</v>
+      </c>
+      <c r="LP15" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1455949</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>06/01/2025</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>SELECCION CANARIA CADETE FEMENINO</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>MADRID CF</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>27</v>
+      </c>
+      <c r="I16" t="n">
+        <v>32</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>3</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" t="n">
+        <v>4</v>
+      </c>
+      <c r="O16" t="n">
+        <v>2</v>
+      </c>
+      <c r="P16" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>3</v>
+      </c>
+      <c r="R16" t="n">
+        <v>9</v>
+      </c>
+      <c r="S16" t="n">
+        <v>6</v>
+      </c>
+      <c r="T16" t="n">
+        <v>12</v>
+      </c>
+      <c r="U16" t="n">
+        <v>11</v>
+      </c>
+      <c r="V16" t="n">
+        <v>15</v>
+      </c>
+      <c r="W16" t="n">
+        <v>15</v>
+      </c>
+      <c r="X16" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>18</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>22</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>24</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>29</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>27</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>32</v>
+      </c>
+      <c r="AH16" t="inlineStr">
+        <is>
+          <t>26:11</t>
+        </is>
+      </c>
+      <c r="AI16" t="inlineStr">
+        <is>
+          <t>14:07</t>
+        </is>
+      </c>
+      <c r="AJ16" t="inlineStr">
+        <is>
+          <t>44:04</t>
+        </is>
+      </c>
+      <c r="AK16" t="inlineStr"/>
+      <c r="AL16" t="inlineStr">
+        <is>
+          <t>52:24</t>
+        </is>
+      </c>
+      <c r="AM16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr">
+        <is>
+          <t>EMMA VERGES MONTES DE OCA</t>
+        </is>
+      </c>
+      <c r="AO16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP16" t="inlineStr"/>
+      <c r="AQ16" t="inlineStr"/>
+      <c r="AR16" t="inlineStr"/>
+      <c r="AS16" t="inlineStr"/>
+      <c r="AT16" t="inlineStr"/>
+      <c r="AU16" t="inlineStr">
+        <is>
+          <t>MARIA GONZALEZ LEON</t>
+        </is>
+      </c>
+      <c r="AV16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW16" t="inlineStr"/>
+      <c r="AX16" t="inlineStr"/>
+      <c r="AY16" t="inlineStr"/>
+      <c r="AZ16" t="inlineStr"/>
+      <c r="BA16" t="inlineStr"/>
+      <c r="BB16" t="inlineStr">
+        <is>
+          <t>LAIA ROY TRULLOLS</t>
+        </is>
+      </c>
+      <c r="BC16" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD16" t="inlineStr"/>
+      <c r="BE16" t="inlineStr">
+        <is>
+          <t>33:37</t>
+        </is>
+      </c>
+      <c r="BF16" t="inlineStr">
+        <is>
+          <t>50:49</t>
+        </is>
+      </c>
+      <c r="BG16" t="inlineStr"/>
+      <c r="BH16" t="inlineStr"/>
+      <c r="BI16" t="inlineStr">
+        <is>
+          <t>JIMENA REDONDO AYLLON</t>
+        </is>
+      </c>
+      <c r="BJ16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK16" t="inlineStr"/>
+      <c r="BL16" t="inlineStr"/>
+      <c r="BM16" t="inlineStr"/>
+      <c r="BN16" t="inlineStr"/>
+      <c r="BO16" t="inlineStr"/>
+      <c r="BP16" t="inlineStr">
+        <is>
+          <t>LAIA VEGAS MARQUES</t>
+        </is>
+      </c>
+      <c r="BQ16" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR16" t="inlineStr"/>
+      <c r="BS16" t="inlineStr"/>
+      <c r="BT16" t="inlineStr"/>
+      <c r="BU16" t="inlineStr"/>
+      <c r="BV16" t="inlineStr"/>
+      <c r="BW16" t="inlineStr">
+        <is>
+          <t>PATRICIA REQUES BERRENDERO</t>
+        </is>
+      </c>
+      <c r="BX16" t="n">
+        <v>7</v>
+      </c>
+      <c r="BY16" t="inlineStr"/>
+      <c r="BZ16" t="inlineStr"/>
+      <c r="CA16" t="inlineStr"/>
+      <c r="CB16" t="inlineStr"/>
+      <c r="CC16" t="inlineStr"/>
+      <c r="CD16" t="inlineStr">
+        <is>
+          <t>ADRIANA MENGUAL ROMERO</t>
+        </is>
+      </c>
+      <c r="CE16" t="n">
+        <v>0</v>
+      </c>
+      <c r="CF16" t="inlineStr"/>
+      <c r="CG16" t="inlineStr"/>
+      <c r="CH16" t="inlineStr"/>
+      <c r="CI16" t="inlineStr"/>
+      <c r="CJ16" t="inlineStr"/>
+      <c r="CK16" t="inlineStr">
+        <is>
+          <t>PAULA GONZALEZ OCHOA</t>
+        </is>
+      </c>
+      <c r="CL16" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM16" t="inlineStr"/>
+      <c r="CN16" t="inlineStr"/>
+      <c r="CO16" t="inlineStr"/>
+      <c r="CP16" t="inlineStr"/>
+      <c r="CQ16" t="inlineStr"/>
+      <c r="CR16" t="inlineStr">
+        <is>
+          <t>BRUNA MIRABAL FERRE</t>
+        </is>
+      </c>
+      <c r="CS16" t="n">
+        <v>0</v>
+      </c>
+      <c r="CT16" t="inlineStr"/>
+      <c r="CU16" t="inlineStr"/>
+      <c r="CV16" t="inlineStr"/>
+      <c r="CW16" t="inlineStr"/>
+      <c r="CX16" t="inlineStr"/>
+      <c r="CY16" t="inlineStr">
+        <is>
+          <t>PAULA RODRIGUEZ RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="CZ16" t="n">
+        <v>4</v>
+      </c>
+      <c r="DA16" t="inlineStr"/>
+      <c r="DB16" t="inlineStr">
+        <is>
+          <t>14:46</t>
+        </is>
+      </c>
+      <c r="DC16" t="inlineStr"/>
+      <c r="DD16" t="inlineStr"/>
+      <c r="DE16" t="inlineStr"/>
+      <c r="DF16" t="inlineStr">
+        <is>
+          <t>AINA SOLER ARASA</t>
+        </is>
+      </c>
+      <c r="DG16" t="n">
+        <v>4</v>
+      </c>
+      <c r="DH16" t="inlineStr"/>
+      <c r="DI16" t="inlineStr"/>
+      <c r="DJ16" t="inlineStr"/>
+      <c r="DK16" t="inlineStr"/>
+      <c r="DL16" t="inlineStr"/>
+      <c r="DM16" t="inlineStr">
+        <is>
+          <t>ELENA SIGUERO GONZALEZ</t>
+        </is>
+      </c>
+      <c r="DN16" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO16" t="inlineStr"/>
+      <c r="DP16" t="inlineStr"/>
+      <c r="DQ16" t="inlineStr"/>
+      <c r="DR16" t="inlineStr"/>
+      <c r="DS16" t="inlineStr"/>
+      <c r="DT16" t="inlineStr">
+        <is>
+          <t>MARTINA NASARRE FRANCO</t>
+        </is>
+      </c>
+      <c r="DU16" t="n">
+        <v>1</v>
+      </c>
+      <c r="DV16" t="inlineStr"/>
+      <c r="DW16" t="inlineStr"/>
+      <c r="DX16" t="inlineStr"/>
+      <c r="DY16" t="inlineStr"/>
+      <c r="DZ16" t="inlineStr"/>
+      <c r="EA16" t="inlineStr">
+        <is>
+          <t>CARLA MONTES ESCRIBANO</t>
+        </is>
+      </c>
+      <c r="EB16" t="n">
+        <v>0</v>
+      </c>
+      <c r="EC16" t="inlineStr"/>
+      <c r="ED16" t="inlineStr"/>
+      <c r="EE16" t="inlineStr"/>
+      <c r="EF16" t="inlineStr"/>
+      <c r="EG16" t="inlineStr"/>
+      <c r="EH16" t="inlineStr">
+        <is>
+          <t>FOIX COLL SOLER</t>
+        </is>
+      </c>
+      <c r="EI16" t="n">
+        <v>0</v>
+      </c>
+      <c r="EJ16" t="inlineStr"/>
+      <c r="EK16" t="inlineStr"/>
+      <c r="EL16" t="inlineStr"/>
+      <c r="EM16" t="inlineStr"/>
+      <c r="EN16" t="inlineStr"/>
+      <c r="EO16" t="inlineStr">
+        <is>
+          <t>SOFIA ATIENZA DE DIEGO</t>
+        </is>
+      </c>
+      <c r="EP16" t="n">
+        <v>0</v>
+      </c>
+      <c r="EQ16" t="inlineStr"/>
+      <c r="ER16" t="inlineStr"/>
+      <c r="ES16" t="inlineStr"/>
+      <c r="ET16" t="inlineStr"/>
+      <c r="EU16" t="inlineStr"/>
+      <c r="EV16" t="inlineStr">
+        <is>
+          <t>MARTINA GONZALEZ ESQUINAS</t>
+        </is>
+      </c>
+      <c r="EW16" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX16" t="inlineStr"/>
+      <c r="EY16" t="inlineStr"/>
+      <c r="EZ16" t="inlineStr"/>
+      <c r="FA16" t="inlineStr"/>
+      <c r="FB16" t="inlineStr"/>
+      <c r="FC16" t="inlineStr">
+        <is>
+          <t>DANIELA MAROTO HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="FD16" t="n">
+        <v>5</v>
+      </c>
+      <c r="FE16" t="inlineStr"/>
+      <c r="FF16" t="inlineStr"/>
+      <c r="FG16" t="inlineStr"/>
+      <c r="FH16" t="inlineStr"/>
+      <c r="FI16" t="inlineStr"/>
+      <c r="FJ16" t="inlineStr">
+        <is>
+          <t>ADRIANA ALSINA ROSELLO</t>
+        </is>
+      </c>
+      <c r="FK16" t="n">
+        <v>0</v>
+      </c>
+      <c r="FL16" t="inlineStr"/>
+      <c r="FM16" t="inlineStr"/>
+      <c r="FN16" t="inlineStr"/>
+      <c r="FO16" t="inlineStr"/>
+      <c r="FP16" t="inlineStr"/>
+      <c r="FQ16" t="inlineStr">
+        <is>
+          <t>CARLA MUNTEANU RUANO</t>
+        </is>
+      </c>
+      <c r="FR16" t="n">
+        <v>0</v>
+      </c>
+      <c r="FS16" t="inlineStr"/>
+      <c r="FT16" t="inlineStr"/>
+      <c r="FU16" t="inlineStr"/>
+      <c r="FV16" t="inlineStr"/>
+      <c r="FW16" t="inlineStr"/>
+      <c r="FX16" t="inlineStr">
+        <is>
+          <t>CANDELA CASTILLA GALLO</t>
+        </is>
+      </c>
+      <c r="FY16" t="n">
+        <v>4</v>
+      </c>
+      <c r="FZ16" t="inlineStr"/>
+      <c r="GA16" t="inlineStr">
+        <is>
+          <t>04:23</t>
+        </is>
+      </c>
+      <c r="GB16" t="inlineStr">
+        <is>
+          <t>39:09</t>
+        </is>
+      </c>
+      <c r="GC16" t="inlineStr">
+        <is>
+          <t>47:26</t>
+        </is>
+      </c>
+      <c r="GD16" t="inlineStr"/>
+      <c r="GE16" t="inlineStr">
+        <is>
+          <t>ROCIO MARTIN MIRANDA</t>
+        </is>
+      </c>
+      <c r="GF16" t="n">
+        <v>0</v>
+      </c>
+      <c r="GG16" t="inlineStr"/>
+      <c r="GH16" t="inlineStr"/>
+      <c r="GI16" t="inlineStr"/>
+      <c r="GJ16" t="inlineStr"/>
+      <c r="GK16" t="inlineStr"/>
+      <c r="GL16" t="inlineStr">
+        <is>
+          <t>LEIRE GUTIERREZ BARQUERO</t>
+        </is>
+      </c>
+      <c r="GM16" t="n">
+        <v>6</v>
+      </c>
+      <c r="GN16" t="inlineStr"/>
+      <c r="GO16" t="inlineStr"/>
+      <c r="GP16" t="inlineStr"/>
+      <c r="GQ16" t="inlineStr"/>
+      <c r="GR16" t="inlineStr"/>
+      <c r="GS16" t="inlineStr">
+        <is>
+          <t>ELSA TESTAL SAN JOSE</t>
+        </is>
+      </c>
+      <c r="GT16" t="n">
+        <v>3</v>
+      </c>
+      <c r="GU16" t="inlineStr"/>
+      <c r="GV16" t="inlineStr"/>
+      <c r="GW16" t="inlineStr"/>
+      <c r="GX16" t="inlineStr"/>
+      <c r="GY16" t="inlineStr"/>
+      <c r="GZ16" t="inlineStr">
+        <is>
+          <t>BERTA BUDED ESPINASA</t>
+        </is>
+      </c>
+      <c r="HA16" t="n">
+        <v>5</v>
+      </c>
+      <c r="HB16" t="inlineStr"/>
+      <c r="HC16" t="inlineStr">
+        <is>
+          <t>41:20</t>
+        </is>
+      </c>
+      <c r="HD16" t="inlineStr"/>
+      <c r="HE16" t="inlineStr"/>
+      <c r="HF16" t="inlineStr"/>
+      <c r="HG16" t="inlineStr">
+        <is>
+          <t>RACHIDA JIREHT ARAGONES OVIEDO</t>
+        </is>
+      </c>
+      <c r="HH16" t="n">
+        <v>0</v>
+      </c>
+      <c r="HI16" t="inlineStr"/>
+      <c r="HJ16" t="inlineStr"/>
+      <c r="HK16" t="inlineStr"/>
+      <c r="HL16" t="inlineStr"/>
+      <c r="HM16" t="inlineStr"/>
+      <c r="HN16" t="inlineStr">
+        <is>
+          <t>SILVIA BENAVENT GONZALEZ</t>
+        </is>
+      </c>
+      <c r="HO16" t="n">
+        <v>2</v>
+      </c>
+      <c r="HP16" t="inlineStr"/>
+      <c r="HQ16" t="inlineStr"/>
+      <c r="HR16" t="inlineStr"/>
+      <c r="HS16" t="inlineStr"/>
+      <c r="HT16" t="inlineStr"/>
+      <c r="HU16" t="inlineStr">
+        <is>
+          <t>DANIELA JIMENEZ LOPEZ</t>
+        </is>
+      </c>
+      <c r="HV16" t="n">
+        <v>5</v>
+      </c>
+      <c r="HW16" t="inlineStr"/>
+      <c r="HX16" t="inlineStr"/>
+      <c r="HY16" t="inlineStr"/>
+      <c r="HZ16" t="inlineStr"/>
+      <c r="IA16" t="inlineStr"/>
+      <c r="IB16" t="inlineStr">
+        <is>
+          <t>LAIA BLAS TORCAL</t>
+        </is>
+      </c>
+      <c r="IC16" t="n">
+        <v>0</v>
+      </c>
+      <c r="ID16" t="inlineStr"/>
+      <c r="IE16" t="inlineStr"/>
+      <c r="IF16" t="inlineStr"/>
+      <c r="IG16" t="inlineStr"/>
+      <c r="IH16" t="inlineStr"/>
+      <c r="II16" t="inlineStr">
+        <is>
+          <t>LUCIA CALLEJA VELASCO</t>
+        </is>
+      </c>
+      <c r="IJ16" t="n">
+        <v>8</v>
+      </c>
+      <c r="IK16" t="inlineStr"/>
+      <c r="IL16" t="inlineStr">
+        <is>
+          <t>41:59</t>
+        </is>
+      </c>
+      <c r="IM16" t="inlineStr"/>
+      <c r="IN16" t="inlineStr"/>
+      <c r="IO16" t="inlineStr"/>
+      <c r="IP16" t="inlineStr">
+        <is>
+          <t>NORA MORELLO LEG</t>
+        </is>
+      </c>
+      <c r="IQ16" t="n">
+        <v>0</v>
+      </c>
+      <c r="IR16" t="inlineStr"/>
+      <c r="IS16" t="inlineStr"/>
+      <c r="IT16" t="inlineStr"/>
+      <c r="IU16" t="inlineStr"/>
+      <c r="IV16" t="inlineStr"/>
+      <c r="IW16" t="inlineStr">
+        <is>
+          <t>CARLA EXPOSITO LOPEZ</t>
+        </is>
+      </c>
+      <c r="IX16" t="n">
+        <v>0</v>
+      </c>
+      <c r="IY16" t="inlineStr"/>
+      <c r="IZ16" t="inlineStr"/>
+      <c r="JA16" t="inlineStr"/>
+      <c r="JB16" t="inlineStr"/>
+      <c r="JC16" t="inlineStr"/>
+      <c r="JD16" t="inlineStr">
+        <is>
+          <t>ENTRENADOR</t>
+        </is>
+      </c>
+      <c r="JE16" t="inlineStr">
+        <is>
+          <t>ERIC BOSSER VIÑAS</t>
+        </is>
+      </c>
+      <c r="JF16" t="inlineStr"/>
+      <c r="JG16" t="inlineStr"/>
+      <c r="JH16" t="inlineStr">
+        <is>
+          <t>AYTE ENTRENADOR</t>
+        </is>
+      </c>
+      <c r="JI16" t="inlineStr">
+        <is>
+          <t>MARTA CANALS I PONS</t>
+        </is>
+      </c>
+      <c r="JJ16" t="inlineStr"/>
+      <c r="JK16" t="inlineStr"/>
+      <c r="JL16" t="inlineStr">
+        <is>
+          <t>OFICIAL</t>
+        </is>
+      </c>
+      <c r="JM16" t="inlineStr">
+        <is>
+          <t>MIRIAM REINA GOMEZ</t>
+        </is>
+      </c>
+      <c r="JN16" t="inlineStr"/>
+      <c r="JO16" t="inlineStr"/>
+      <c r="JP16" t="inlineStr">
+        <is>
+          <t>OFICIAL</t>
+        </is>
+      </c>
+      <c r="JQ16" t="inlineStr">
+        <is>
+          <t>RAQUEL MARTINEZ REVIEJO</t>
+        </is>
+      </c>
+      <c r="JR16" t="inlineStr"/>
+      <c r="JS16" t="inlineStr"/>
+      <c r="JT16" t="inlineStr"/>
+      <c r="JU16" t="inlineStr"/>
+      <c r="JV16" t="inlineStr"/>
+      <c r="JW16" t="inlineStr"/>
+      <c r="JX16" t="n">
+        <v>59</v>
+      </c>
+      <c r="JY16" t="n">
+        <v>-5</v>
+      </c>
+      <c r="JZ16" t="n">
+        <v>5</v>
+      </c>
+      <c r="KA16" t="n">
+        <v>6</v>
+      </c>
+      <c r="KB16" t="n">
+        <v>2</v>
+      </c>
+      <c r="KC16" t="n">
+        <v>2</v>
+      </c>
+      <c r="KD16" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE16" t="n">
+        <v>1</v>
+      </c>
+      <c r="KF16" t="n">
+        <v>1</v>
+      </c>
+      <c r="KG16" t="n">
+        <v>1</v>
+      </c>
+      <c r="KH16" t="n">
+        <v>1</v>
+      </c>
+      <c r="KI16" t="n">
+        <v>3</v>
+      </c>
+      <c r="KJ16" t="n">
+        <v>1</v>
+      </c>
+      <c r="KK16" t="n">
+        <v>2</v>
+      </c>
+      <c r="KL16" t="n">
+        <v>3</v>
+      </c>
+      <c r="KM16" t="n">
+        <v>3</v>
+      </c>
+      <c r="KN16" t="n">
+        <v>5</v>
+      </c>
+      <c r="KO16" t="n">
+        <v>3</v>
+      </c>
+      <c r="KP16" t="n">
+        <v>4</v>
+      </c>
+      <c r="KQ16" t="n">
+        <v>3</v>
+      </c>
+      <c r="KR16" t="n">
+        <v>3</v>
+      </c>
+      <c r="KS16" t="n">
+        <v>2</v>
+      </c>
+      <c r="KT16" t="n">
+        <v>4</v>
+      </c>
+      <c r="KU16" t="n">
+        <v>2</v>
+      </c>
+      <c r="KV16" t="n">
+        <v>3</v>
+      </c>
+      <c r="KW16" t="n">
+        <v>2</v>
+      </c>
+      <c r="KX16" t="n">
+        <v>4</v>
+      </c>
+      <c r="KY16" t="n">
+        <v>3</v>
+      </c>
+      <c r="KZ16" t="n">
+        <v>3</v>
+      </c>
+      <c r="LA16" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LB16" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LC16" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LD16" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LE16" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LF16" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LG16" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LH16" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LI16" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LJ16" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LK16" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LL16" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="LM16" t="inlineStr">
+        <is>
+          <t>Local</t>
+        </is>
+      </c>
+      <c r="LN16" t="inlineStr">
+        <is>
+          <t>Visitante</t>
+        </is>
+      </c>
+      <c r="LO16" t="n">
+        <v>2</v>
+      </c>
+      <c r="LP16" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>